<commit_message>
data update. pul mithai and janpath
</commit_message>
<xml_diff>
--- a/data/Workbook_edited.xlsx
+++ b/data/Workbook_edited.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandakmayank/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandakmayank/missingbasti/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="4060" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="2700" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="459">
   <si>
     <t>headline</t>
   </si>
@@ -1379,12 +1379,48 @@
   <si>
     <t>img/kidwai/audio.mp3</t>
   </si>
+  <si>
+    <t>SUBODH</t>
+  </si>
+  <si>
+    <t>Still recovering from the loss of her husband’s death, Mangala has geared up to fight a new war with the eviction, rains, and winter. All her belongings are ruined by rain and children dropped out of school. She complains about the Railway police confiscating their belongings and not reluctant on returning it back.</t>
+  </si>
+  <si>
+    <t>“I got really scared when I heard the noises at 07:00 am in the morning. Not informed about the eviction, I had no option to save my belongings as I was removing my children from the affected spot.” She has already submitted a copy of her Aadhar card and voter Id to the activists demanding aid and a stay order.</t>
+  </si>
+  <si>
+    <t>Subodh points out to a burst water pipeline near the railway tracks, with a single stream of water spraying as the only source of water for 270 families in that area. Inaccessible public toilets (200 m away, across the railway tracks) are the reason people practice open defecation. He is thankful to the NGOs, who contribute to the education of the children in the Basti, although the number of dropouts is large every month.</t>
+  </si>
+  <si>
+    <t>img/pul_mithai/mangala.jpg</t>
+  </si>
+  <si>
+    <t>img/pul_mithai/Mariam.jpg</t>
+  </si>
+  <si>
+    <t>img/pul_mithai/Subodh.jpg</t>
+  </si>
+  <si>
+    <t>MANGALA. From Darbhanga (Bihar)</t>
+  </si>
+  <si>
+    <t>MARIAM. From Bhagalpur (Bihar)</t>
+  </si>
+  <si>
+    <t>img/janpath/pradhan.jpg</t>
+  </si>
+  <si>
+    <t>img/janpath/madan.jpg</t>
+  </si>
+  <si>
+    <t>img/janpath/suresh.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1461,6 +1497,23 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FFCC0000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFCC0000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1500,7 +1553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1569,6 +1622,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1848,9 +1910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AW3" sqref="AW3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2270,15 +2332,33 @@
       <c r="AM2" s="11">
         <v>2017</v>
       </c>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10"/>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="10"/>
+      <c r="AN2" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="AO2" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="AP2" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="AR2" s="27" t="s">
+        <v>455</v>
+      </c>
+      <c r="AS2" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="AT2" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="AU2" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="AV2" s="28" t="s">
+        <v>450</v>
+      </c>
       <c r="AW2" s="3"/>
     </row>
     <row r="3" spans="1:191" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2393,31 +2473,31 @@
       <c r="AM3" s="12">
         <v>2010</v>
       </c>
-      <c r="AN3" s="11" t="s">
+      <c r="AN3" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="AO3" s="18" t="s">
+      <c r="AO3" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="AP3" s="19" t="s">
+      <c r="AP3" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="AR3" s="18" t="s">
+      <c r="AR3" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="AS3" s="19" t="s">
+      <c r="AS3" s="30" t="s">
         <v>328</v>
       </c>
-      <c r="AT3" s="11" t="s">
+      <c r="AT3" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="AU3" s="18" t="s">
+      <c r="AU3" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="AV3" s="19" t="s">
+      <c r="AV3" s="30" t="s">
         <v>329</v>
       </c>
       <c r="AW3" s="20" t="s">
@@ -3440,15 +3520,33 @@
         <v>209</v>
       </c>
       <c r="AM9" s="10"/>
-      <c r="AN9" s="10"/>
-      <c r="AO9" s="10"/>
-      <c r="AP9" s="10"/>
-      <c r="AQ9" s="10"/>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="10"/>
-      <c r="AT9" s="10"/>
-      <c r="AU9" s="10"/>
-      <c r="AV9" s="10"/>
+      <c r="AN9" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="AO9" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="AP9" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="AQ9" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="AR9" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="AS9" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="AT9" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="AU9" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="AV9" s="19" t="s">
+        <v>329</v>
+      </c>
       <c r="AW9" s="3"/>
       <c r="AX9"/>
       <c r="AY9"/>

</xml_diff>